<commit_message>
Enhance document and user APIs with improved response structures, implement vector similarity search, and update authentication flow. Add tests for document chunk retrieval and searching.
</commit_message>
<xml_diff>
--- a/db_schema.xlsx
+++ b/db_schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -82,6 +82,18 @@
     <t xml:space="preserve">Hashed password</t>
   </si>
   <si>
+    <t xml:space="preserve">is_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is admin user</t>
+  </si>
+  <si>
     <t xml:space="preserve">created_at</t>
   </si>
   <si>
@@ -91,6 +103,12 @@
     <t xml:space="preserve">User creation timestamp</t>
   </si>
   <si>
+    <t xml:space="preserve">updated_at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User update timestamp</t>
+  </si>
+  <si>
     <t xml:space="preserve">documents</t>
   </si>
   <si>
@@ -124,6 +142,9 @@
     <t xml:space="preserve">Document creation timestamp</t>
   </si>
   <si>
+    <t xml:space="preserve">Document update timestamp</t>
+  </si>
+  <si>
     <t xml:space="preserve">document_chunks</t>
   </si>
   <si>
@@ -161,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">Chunk creation timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chunk update timestamp</t>
   </si>
   <si>
     <t xml:space="preserve">status</t>
@@ -371,10 +395,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,75 +500,75 @@
         <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
@@ -555,101 +579,101 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>44</v>
@@ -660,36 +684,104 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>